<commit_message>
Test référence double 116abf50bfd3126e0e0d8e3c02488c45a2f1803b
</commit_message>
<xml_diff>
--- a/ML/ig/StructureDefinition-PersonnePriseCharge.xlsx
+++ b/ML/ig/StructureDefinition-PersonnePriseCharge.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-30T16:36:55+00:00</t>
+    <t>2025-10-30T16:59:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2563,7 +2563,7 @@
         <v>72</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>71</v>
@@ -2638,7 +2638,7 @@
         <v>72</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>71</v>

</xml_diff>